<commit_message>
modify sub-items in the left panel
</commit_message>
<xml_diff>
--- a/inst/hidap_agrofims/PURI1567089918.xlsx
+++ b/inst/hidap_agrofims/PURI1567089918.xlsx
@@ -21,8 +21,8 @@
     <sheet name="Phenology" sheetId="12" r:id="rId12"/>
     <sheet name="Soil" sheetId="13" r:id="rId13"/>
     <sheet name="TraitList" sheetId="14" r:id="rId14"/>
-    <sheet name="Stress_management" sheetId="15" r:id="rId15"/>
-    <sheet name="Unexpected" sheetId="16" r:id="rId16"/>
+    <sheet name="Unexpected" sheetId="15" r:id="rId15"/>
+    <sheet name="Stress_management" sheetId="16" r:id="rId16"/>
     <sheet name="for_analysis" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1172,12 +1172,12 @@
     <t>PLOT</t>
   </si>
   <si>
+    <t>strong rain</t>
+  </si>
+  <si>
     <t>disease</t>
   </si>
   <si>
-    <t>strong rain</t>
-  </si>
-  <si>
     <t>fungus on maize</t>
   </si>
   <si>
@@ -1763,6 +1763,24 @@
     <t>Aerial applicator|Airblast sprayer|Backpack sprayer|Boom sprayer|Duster|Electrostatic sprayer|Fogger|Hand sprayer|Injection sprayer|Mist blower|Recirculating sprayer|Seed treater|Tree injector|Wiper|Other|.*</t>
   </si>
   <si>
+    <t>new trait for marie__1</t>
+  </si>
+  <si>
+    <t>TIMESTAMP_new trait for marie__1</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>salut</t>
+  </si>
+  <si>
+    <t>Ola</t>
+  </si>
+  <si>
+    <t>hallo</t>
+  </si>
+  <si>
     <t>Biotic_stress_control_product_amount_g/m2__1</t>
   </si>
   <si>
@@ -1778,22 +1796,13 @@
     <t>7.00</t>
   </si>
   <si>
-    <t>new trait for marie__1</t>
-  </si>
-  <si>
-    <t>TIMESTAMP_new trait for marie__1</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>salut</t>
-  </si>
-  <si>
-    <t>Ola</t>
-  </si>
-  <si>
-    <t>hallo</t>
+    <t>2:Soil_porosity_%__2</t>
+  </si>
+  <si>
+    <t>TIMESTAMP_2:Soil_porosity_%__2</t>
+  </si>
+  <si>
+    <t>63.00</t>
   </si>
   <si>
     <t>1:Soil_porosity_%__1</t>
@@ -1805,19 +1814,10 @@
     <t>64.00</t>
   </si>
   <si>
-    <t>63.00</t>
-  </si>
-  <si>
-    <t>2:Soil_porosity_%__2</t>
-  </si>
-  <si>
-    <t>TIMESTAMP_2:Soil_porosity_%__2</t>
+    <t>disease_Notes_Deviations</t>
   </si>
   <si>
     <t>strong rain_Notes_Deviations</t>
-  </si>
-  <si>
-    <t>disease_Notes_Deviations</t>
   </si>
 </sst>
 </file>
@@ -7044,6 +7044,179 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E2" t="s">
+        <v>579</v>
+      </c>
+      <c r="F2" t="s">
+        <v>346</v>
+      </c>
+      <c r="G2" t="s">
+        <v>590</v>
+      </c>
+      <c r="H2" t="s">
+        <v>414</v>
+      </c>
+      <c r="I2" t="s">
+        <v>593</v>
+      </c>
+      <c r="J2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>400</v>
+      </c>
+      <c r="E3" t="s">
+        <v>580</v>
+      </c>
+      <c r="F3" t="s">
+        <v>346</v>
+      </c>
+      <c r="G3" t="s">
+        <v>402</v>
+      </c>
+      <c r="H3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I3" t="s">
+        <v>437</v>
+      </c>
+      <c r="J3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>399</v>
+      </c>
+      <c r="E4" t="s">
+        <v>581</v>
+      </c>
+      <c r="F4" t="s">
+        <v>346</v>
+      </c>
+      <c r="G4" t="s">
+        <v>405</v>
+      </c>
+      <c r="H4" t="s">
+        <v>414</v>
+      </c>
+      <c r="I4" t="s">
+        <v>590</v>
+      </c>
+      <c r="J4" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>400</v>
+      </c>
+      <c r="E5" t="s">
+        <v>582</v>
+      </c>
+      <c r="F5" t="s">
+        <v>346</v>
+      </c>
+      <c r="G5" t="s">
+        <v>439</v>
+      </c>
+      <c r="H5" t="s">
+        <v>414</v>
+      </c>
+      <c r="I5" t="s">
+        <v>590</v>
+      </c>
+      <c r="J5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7064,10 +7237,10 @@
         <v>386</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>577</v>
+        <v>583</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -7104,7 +7277,7 @@
         <v>400</v>
       </c>
       <c r="E3" t="s">
-        <v>579</v>
+        <v>585</v>
       </c>
       <c r="F3" t="s">
         <v>346</v>
@@ -7124,7 +7297,7 @@
         <v>399</v>
       </c>
       <c r="E4" t="s">
-        <v>580</v>
+        <v>586</v>
       </c>
       <c r="F4" t="s">
         <v>346</v>
@@ -7144,183 +7317,10 @@
         <v>400</v>
       </c>
       <c r="E5" t="s">
-        <v>581</v>
+        <v>587</v>
       </c>
       <c r="F5" t="s">
         <v>346</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>592</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>399</v>
-      </c>
-      <c r="E2" t="s">
-        <v>584</v>
-      </c>
-      <c r="F2" t="s">
-        <v>346</v>
-      </c>
-      <c r="G2" t="s">
-        <v>590</v>
-      </c>
-      <c r="H2" t="s">
-        <v>414</v>
-      </c>
-      <c r="I2" t="s">
-        <v>591</v>
-      </c>
-      <c r="J2" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>400</v>
-      </c>
-      <c r="E3" t="s">
-        <v>585</v>
-      </c>
-      <c r="F3" t="s">
-        <v>346</v>
-      </c>
-      <c r="G3" t="s">
-        <v>437</v>
-      </c>
-      <c r="H3" t="s">
-        <v>414</v>
-      </c>
-      <c r="I3" t="s">
-        <v>402</v>
-      </c>
-      <c r="J3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>399</v>
-      </c>
-      <c r="E4" t="s">
-        <v>586</v>
-      </c>
-      <c r="F4" t="s">
-        <v>346</v>
-      </c>
-      <c r="G4" t="s">
-        <v>591</v>
-      </c>
-      <c r="H4" t="s">
-        <v>414</v>
-      </c>
-      <c r="I4" t="s">
-        <v>405</v>
-      </c>
-      <c r="J4" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>400</v>
-      </c>
-      <c r="E5" t="s">
-        <v>587</v>
-      </c>
-      <c r="F5" t="s">
-        <v>346</v>
-      </c>
-      <c r="G5" t="s">
-        <v>591</v>
-      </c>
-      <c r="H5" t="s">
-        <v>414</v>
-      </c>
-      <c r="I5" t="s">
-        <v>439</v>
-      </c>
-      <c r="J5" t="s">
-        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -7428,10 +7428,10 @@
         <v>578</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>588</v>
@@ -7440,10 +7440,10 @@
         <v>589</v>
       </c>
       <c r="AI1" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>592</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>593</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>178</v>
@@ -7709,13 +7709,13 @@
         <v>438</v>
       </c>
       <c r="AC2" t="s">
-        <v>419</v>
+        <v>579</v>
       </c>
       <c r="AD2" t="s">
         <v>346</v>
       </c>
       <c r="AE2" t="s">
-        <v>584</v>
+        <v>419</v>
       </c>
       <c r="AF2" t="s">
         <v>346</v>
@@ -7727,7 +7727,7 @@
         <v>414</v>
       </c>
       <c r="AI2" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="AJ2" t="s">
         <v>414</v>
@@ -7990,7 +7990,7 @@
         <v>405</v>
       </c>
       <c r="AC3" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="AD3" t="s">
         <v>346</v>
@@ -8002,13 +8002,13 @@
         <v>346</v>
       </c>
       <c r="AG3" t="s">
-        <v>437</v>
+        <v>402</v>
       </c>
       <c r="AH3" t="s">
         <v>414</v>
       </c>
       <c r="AI3" t="s">
-        <v>402</v>
+        <v>437</v>
       </c>
       <c r="AJ3" t="s">
         <v>414</v>
@@ -8271,7 +8271,7 @@
         <v>439</v>
       </c>
       <c r="AC4" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="AD4" t="s">
         <v>346</v>
@@ -8283,13 +8283,13 @@
         <v>346</v>
       </c>
       <c r="AG4" t="s">
-        <v>591</v>
+        <v>405</v>
       </c>
       <c r="AH4" t="s">
         <v>414</v>
       </c>
       <c r="AI4" t="s">
-        <v>405</v>
+        <v>590</v>
       </c>
       <c r="AJ4" t="s">
         <v>414</v>
@@ -8477,8 +8477,8 @@
       <c r="CS4" t="s">
         <v>376</v>
       </c>
-      <c r="CT4" t="s">
-        <v>381</v>
+      <c r="CU4" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="5" spans="1:99">
@@ -8555,7 +8555,7 @@
         <v>440</v>
       </c>
       <c r="AC5" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="AD5" t="s">
         <v>346</v>
@@ -8567,13 +8567,13 @@
         <v>346</v>
       </c>
       <c r="AG5" t="s">
-        <v>591</v>
+        <v>439</v>
       </c>
       <c r="AH5" t="s">
         <v>414</v>
       </c>
       <c r="AI5" t="s">
-        <v>439</v>
+        <v>590</v>
       </c>
       <c r="AJ5" t="s">
         <v>414</v>
@@ -8761,8 +8761,8 @@
       <c r="CS5" t="s">
         <v>376</v>
       </c>
-      <c r="CU5" t="s">
-        <v>380</v>
+      <c r="CT5" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -11438,19 +11438,19 @@
       <c r="A2" t="s">
         <v>380</v>
       </c>
-      <c r="B2" t="s">
-        <v>382</v>
-      </c>
       <c r="C2" t="s">
-        <v>383</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>381</v>
       </c>
+      <c r="B3" t="s">
+        <v>382</v>
+      </c>
       <c r="C3" t="s">
-        <v>348</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix file path for test version 26
</commit_message>
<xml_diff>
--- a/inst/hidap_agrofims/PURI1567089918.xlsx
+++ b/inst/hidap_agrofims/PURI1567089918.xlsx
@@ -1763,6 +1763,33 @@
     <t>Aerial applicator|Airblast sprayer|Backpack sprayer|Boom sprayer|Duster|Electrostatic sprayer|Fogger|Hand sprayer|Injection sprayer|Mist blower|Recirculating sprayer|Seed treater|Tree injector|Wiper|Other|.*</t>
   </si>
   <si>
+    <t>1:Soil_porosity_%__1</t>
+  </si>
+  <si>
+    <t>TIMESTAMP_1:Soil_porosity_%__1</t>
+  </si>
+  <si>
+    <t>64.00</t>
+  </si>
+  <si>
+    <t>63.00</t>
+  </si>
+  <si>
+    <t>Biotic_stress_control_product_amount_g/m2__1</t>
+  </si>
+  <si>
+    <t>TIMESTAMP_Biotic_stress_control_product_amount_g/m2__1</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>88.00</t>
+  </si>
+  <si>
+    <t>7.00</t>
+  </si>
+  <si>
     <t>new trait for marie__1</t>
   </si>
   <si>
@@ -1781,37 +1808,10 @@
     <t>hallo</t>
   </si>
   <si>
-    <t>Biotic_stress_control_product_amount_g/m2__1</t>
-  </si>
-  <si>
-    <t>TIMESTAMP_Biotic_stress_control_product_amount_g/m2__1</t>
-  </si>
-  <si>
-    <t>2.00</t>
-  </si>
-  <si>
-    <t>88.00</t>
-  </si>
-  <si>
-    <t>7.00</t>
-  </si>
-  <si>
     <t>2:Soil_porosity_%__2</t>
   </si>
   <si>
     <t>TIMESTAMP_2:Soil_porosity_%__2</t>
-  </si>
-  <si>
-    <t>63.00</t>
-  </si>
-  <si>
-    <t>1:Soil_porosity_%__1</t>
-  </si>
-  <si>
-    <t>TIMESTAMP_1:Soil_porosity_%__1</t>
-  </si>
-  <si>
-    <t>64.00</t>
   </si>
   <si>
     <t>disease_Notes_Deviations</t>
@@ -7044,13 +7044,13 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>379</v>
       </c>
@@ -7070,19 +7070,13 @@
         <v>578</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>591</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7099,22 +7093,16 @@
         <v>579</v>
       </c>
       <c r="F2" t="s">
-        <v>346</v>
+        <v>414</v>
       </c>
       <c r="G2" t="s">
-        <v>590</v>
+        <v>580</v>
       </c>
       <c r="H2" t="s">
         <v>414</v>
       </c>
-      <c r="I2" t="s">
-        <v>593</v>
-      </c>
-      <c r="J2" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7128,10 +7116,10 @@
         <v>400</v>
       </c>
       <c r="E3" t="s">
-        <v>580</v>
+        <v>437</v>
       </c>
       <c r="F3" t="s">
-        <v>346</v>
+        <v>414</v>
       </c>
       <c r="G3" t="s">
         <v>402</v>
@@ -7139,14 +7127,8 @@
       <c r="H3" t="s">
         <v>414</v>
       </c>
-      <c r="I3" t="s">
-        <v>437</v>
-      </c>
-      <c r="J3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7160,10 +7142,10 @@
         <v>399</v>
       </c>
       <c r="E4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F4" t="s">
-        <v>346</v>
+        <v>414</v>
       </c>
       <c r="G4" t="s">
         <v>405</v>
@@ -7171,14 +7153,8 @@
       <c r="H4" t="s">
         <v>414</v>
       </c>
-      <c r="I4" t="s">
-        <v>590</v>
-      </c>
-      <c r="J4" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7192,21 +7168,15 @@
         <v>400</v>
       </c>
       <c r="E5" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F5" t="s">
-        <v>346</v>
+        <v>414</v>
       </c>
       <c r="G5" t="s">
         <v>439</v>
       </c>
       <c r="H5" t="s">
-        <v>414</v>
-      </c>
-      <c r="I5" t="s">
-        <v>590</v>
-      </c>
-      <c r="J5" t="s">
         <v>414</v>
       </c>
     </row>
@@ -7217,13 +7187,13 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>379</v>
       </c>
@@ -7237,13 +7207,19 @@
         <v>386</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>582</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7262,8 +7238,14 @@
       <c r="F2" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>588</v>
+      </c>
+      <c r="H2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7277,13 +7259,19 @@
         <v>400</v>
       </c>
       <c r="E3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="F3" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>589</v>
+      </c>
+      <c r="H3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7297,13 +7285,19 @@
         <v>399</v>
       </c>
       <c r="E4" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="F4" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="s">
+        <v>590</v>
+      </c>
+      <c r="H4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7317,9 +7311,15 @@
         <v>400</v>
       </c>
       <c r="E5" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F5" t="s">
+        <v>346</v>
+      </c>
+      <c r="G5" t="s">
+        <v>591</v>
+      </c>
+      <c r="H5" t="s">
         <v>346</v>
       </c>
     </row>
@@ -7428,22 +7428,22 @@
         <v>578</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>178</v>
@@ -7712,7 +7712,7 @@
         <v>579</v>
       </c>
       <c r="AD2" t="s">
-        <v>346</v>
+        <v>414</v>
       </c>
       <c r="AE2" t="s">
         <v>419</v>
@@ -7721,13 +7721,13 @@
         <v>346</v>
       </c>
       <c r="AG2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="AH2" t="s">
-        <v>414</v>
+        <v>346</v>
       </c>
       <c r="AI2" t="s">
-        <v>593</v>
+        <v>580</v>
       </c>
       <c r="AJ2" t="s">
         <v>414</v>
@@ -7990,25 +7990,25 @@
         <v>405</v>
       </c>
       <c r="AC3" t="s">
-        <v>580</v>
+        <v>437</v>
       </c>
       <c r="AD3" t="s">
-        <v>346</v>
+        <v>414</v>
       </c>
       <c r="AE3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="AF3" t="s">
         <v>346</v>
       </c>
       <c r="AG3" t="s">
+        <v>589</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>346</v>
+      </c>
+      <c r="AI3" t="s">
         <v>402</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>414</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>437</v>
       </c>
       <c r="AJ3" t="s">
         <v>414</v>
@@ -8271,25 +8271,25 @@
         <v>439</v>
       </c>
       <c r="AC4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="AD4" t="s">
-        <v>346</v>
+        <v>414</v>
       </c>
       <c r="AE4" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="AF4" t="s">
         <v>346</v>
       </c>
       <c r="AG4" t="s">
+        <v>590</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>346</v>
+      </c>
+      <c r="AI4" t="s">
         <v>405</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>414</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>590</v>
       </c>
       <c r="AJ4" t="s">
         <v>414</v>
@@ -8555,25 +8555,25 @@
         <v>440</v>
       </c>
       <c r="AC5" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="AD5" t="s">
-        <v>346</v>
+        <v>414</v>
       </c>
       <c r="AE5" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="AF5" t="s">
         <v>346</v>
       </c>
       <c r="AG5" t="s">
+        <v>591</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>346</v>
+      </c>
+      <c r="AI5" t="s">
         <v>439</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>414</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>590</v>
       </c>
       <c r="AJ5" t="s">
         <v>414</v>

</xml_diff>